<commit_message>
Handle select tags and handle multilpe fields per accession
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elilu\code\esbase-automation-scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C38848BB-9328-44E8-BCEB-EE281E8C9020}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E895CF4-1BB3-4D4F-B3C9-3D29D1ECCCA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" xr2:uid="{E6C9AF9F-5941-40A4-BFFE-294BD35F2B30}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{E6C9AF9F-5941-40A4-BFFE-294BD35F2B30}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,21 +36,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>accnr</t>
   </si>
   <si>
-    <t>property_id</t>
-  </si>
-  <si>
-    <t>new_value</t>
-  </si>
-  <si>
-    <t>table_Accession_Note</t>
-  </si>
-  <si>
-    <t>Ingår i serie: B2023/04725-04797</t>
+    <t>catalogBlock_Fish_GenderId</t>
+  </si>
+  <si>
+    <t>Hona</t>
+  </si>
+  <si>
+    <t>property_id2</t>
+  </si>
+  <si>
+    <t>property_id1</t>
+  </si>
+  <si>
+    <t>new_value1</t>
+  </si>
+  <si>
+    <t>new_value2</t>
+  </si>
+  <si>
+    <t>catalogBlock_Fish_Totallength</t>
   </si>
 </sst>
 </file>
@@ -402,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{583C0FD4-C008-4862-966D-D712A9AB07F8}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -413,28 +422,42 @@
     <col min="1" max="1" width="25.1328125" customWidth="1"/>
     <col min="2" max="2" width="27.1328125" customWidth="1"/>
     <col min="3" max="3" width="36.73046875" customWidth="1"/>
+    <col min="4" max="4" width="31.33203125" customWidth="1"/>
+    <col min="5" max="5" width="31.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A2">
+        <v>202201037</v>
+      </c>
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A2">
-        <v>202301111</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2">
+        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update example to new accnr format in excel
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elilu\code\esbase-automation-scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E895CF4-1BB3-4D4F-B3C9-3D29D1ECCCA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28E3B791-7304-49A3-AFFE-EE1AF775CAFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{E6C9AF9F-5941-40A4-BFFE-294BD35F2B30}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" xr2:uid="{E6C9AF9F-5941-40A4-BFFE-294BD35F2B30}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
   <si>
     <t>accnr</t>
   </si>
@@ -60,6 +60,12 @@
   </si>
   <si>
     <t>catalogBlock_Fish_Totallength</t>
+  </si>
+  <si>
+    <t>A2022/12345</t>
+  </si>
+  <si>
+    <t>A202212345</t>
   </si>
 </sst>
 </file>
@@ -411,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{583C0FD4-C008-4862-966D-D712A9AB07F8}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -444,8 +450,8 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A2">
-        <v>202201037</v>
+      <c r="A2" t="s">
+        <v>8</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -457,6 +463,23 @@
         <v>7</v>
       </c>
       <c r="E2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3">
         <v>123</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update example to new select which is based on value
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elilu\code\esbase-automation-scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28E3B791-7304-49A3-AFFE-EE1AF775CAFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB16DDA5-67EF-469C-9CCE-CEDD385F9ACC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" xr2:uid="{E6C9AF9F-5941-40A4-BFFE-294BD35F2B30}"/>
   </bookViews>
@@ -36,15 +36,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>accnr</t>
   </si>
   <si>
     <t>catalogBlock_Fish_GenderId</t>
-  </si>
-  <si>
-    <t>Hona</t>
   </si>
   <si>
     <t>property_id2</t>
@@ -420,7 +417,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -437,30 +434,30 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
         <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
-        <v>2</v>
+      <c r="C2">
+        <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E2">
         <v>123</v>
@@ -468,16 +465,16 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
-        <v>2</v>
+      <c r="C3">
+        <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E3">
         <v>123</v>

</xml_diff>